<commit_message>
Automatische sync: 2025-06-17 09:57:34
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,8 +684,72 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-17 08:58:06</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-17 09:28:13</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -705,7 +769,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -723,7 +787,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -753,6 +817,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 10:57:36
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,8 +748,47 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 uur tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 uur tot 16:00 uur. Voor eventuele feestdagen en afwijkende openingstijden, adviseer ik onze website te raadplegen.
+Met vriendelijke groet, [Jouw naam]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-17 10:28:27</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -769,7 +808,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -787,7 +826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -837,6 +876,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 11:57:38
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,8 +787,82 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-17 10:58:37</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 uur tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 uur tot 16:00 uur. Voor eventuele feestdagen en afwijkende openingstijden, adviseer ik onze website te raadplegen.
+Met vriendelijke groet, [Jouw naam]</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste,
+Hartelijk dank voor uw interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 uur tot 18:00 uur en op zaterdag van 10:00 uur tot 16:00 uur. Voor eventuele feestdagen en afwijkende openingstijden kunt u onze website raadplegen.
+Met vriendelijke groet,
+[Jouw naam]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-17 10:58:40</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -808,7 +882,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -826,7 +900,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,17 +923,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Informatieaanvraag</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -869,7 +943,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -879,10 +953,20 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Informatieaanvraag</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 12:57:39
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,8 +861,123 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-17 11:59:01</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor uw interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 tot 16:00 uur. Op zondag zijn wij gesloten. Mocht u verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-17 11:59:03</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor uw interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 tot 16:00 uur. Op zondag zijn wij gesloten. Mocht u verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw interesse. Onze openingstijden zijn maandag t/m vrijdag van 9:00 tot 18:00 uur en zaterdag van 10:00 tot 16:00 uur. Op zondag zijn wij gesloten. Voor verdere vragen kunt u altijd contact met ons opnemen.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-17 12:29:15</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -882,7 +997,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -927,23 +1042,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -963,7 +1078,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 13:57:41
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -976,8 +976,158 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Re: Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw interesse. Onze openingstijden zijn maandag t/m vrijdag van 9:00 tot 18:00 uur en zaterdag van 10:00 tot 16:00 uur. Op zondag zijn wij gesloten. Voor verdere vragen kunt u altijd contact met ons opnemen.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank voor uw interesse. Wij zijn geopend op maandag t/m vrijdag van 9:00-18:00 en zaterdag van 10:00-16:00. Op zondag zijn wij gesloten. Voor vragen zijn wij bereikbaar via info@bedrijfsnaam.nl of telefonisch op [telefoonnummer]. 
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-17 12:59:24</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-17 12:59:24</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-17 12:59:25</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Re: Re: Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank voor uw interesse. Wij zijn geopend op maandag t/m vrijdag van 9:00-18:00 en zaterdag van 10:00-16:00. Op zondag zijn wij gesloten. Voor vragen zijn wij bereikbaar via info@bedrijfsnaam.nl of telefonisch op [telefoonnummer]. 
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw interesse. Onze openingstijden zijn ma t/m vr van 9:00-18:00 en za van 10:00-16:00. Op zondag zijn we gesloten. Voor vragen zijn we bereikbaar via info@bedrijfsnaam.nl of telefonisch op [telefoonnummer].
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-17 13:29:35</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -997,7 +1147,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1042,27 +1192,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 14:57:43
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1126,8 +1126,115 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Re: Re: Re: Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw interesse. Onze openingstijden zijn ma t/m vr van 9:00-18:00 en za van 10:00-16:00. Op zondag zijn we gesloten. Voor vragen zijn we bereikbaar via info@bedrijfsnaam.nl of telefonisch op [telefoonnummer].
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank voor uw bericht. Onze openingstijden zijn ma t/m vr van 9:00-18:00 en za van 10:00-16:00. Op zondag zijn wij gesloten. Voor vragen zijn wij bereikbaar via info@bedrijfsnaam.nl of telefonisch op [telefoonnummer].
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-17 13:59:44</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-17 13:59:45</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-17 14:29:52</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1147,7 +1254,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1192,7 +1299,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -1202,7 +1309,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -1212,7 +1319,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 15:57:44
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,8 +1233,40 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-17 14:59:58</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1254,7 +1286,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1309,7 +1341,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 16:57:46
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1265,8 +1265,72 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-17 16:00:10</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-17 16:30:23</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1286,7 +1350,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1341,7 +1405,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -1357,17 +1421,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische sync: 2025-06-17 20:41:37
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1329,8 +1329,92 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Hallo, ik wil graag weten wanneer jullie bereikbaar zijn.
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Onze kantooruren zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Buiten deze tijden proberen we zo snel mogelijk te reageren. Mocht je verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-17 20:40:26</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Onze kantooruren zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Buiten deze tijden proberen we zo snel mogelijk te reageren. Mocht je verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-17 20:40:38</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1350,7 +1434,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1395,7 +1479,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:34:45
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1413,8 +1413,180 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Re: Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-17 20:44:19</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Re: Re: Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar een spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-06-17 20:44:34</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Re: Re: Re: Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar een spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar een spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-17 20:46:24</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Re: Re: Re: Re: Re: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar een spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Dank voor je bericht. Onze kantooruren zijn van maandag t/m vrijdag van 9:00-17:00 uur. Buiten deze tijden streven we naar een spoedige reactie. Voor verdere vragen, neem gerust contact met ons op.
+Met vriendelijke groet,
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-17 20:46:41</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1434,7 +1606,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1479,7 +1651,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:37:03
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1585,8 +1585,40 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:36:58</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1606,7 +1638,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1677,7 +1709,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1687,11 +1719,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:40:09
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1617,8 +1617,80 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:39:10</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je bericht. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 uur tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 uur tot 14:00 uur. Zondag zijn wij gesloten. Mocht je nog vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,  
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:39:12</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1638,7 +1710,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1683,7 +1755,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -1699,7 +1771,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1709,11 +1781,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:41:12
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1689,8 +1689,40 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:40:19</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1710,7 +1742,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1771,17 +1803,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:49:25
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1721,8 +1721,80 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 18:00 uur. Op zaterdag zijn we geopend van 10:00 tot 16:00 uur. Op zondag zijn we gesloten. Mocht je nog vragen hebben, dan hoor ik het graag.
+Met vriendelijke groet,
+[Naam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:49:20</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:49:21</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1742,7 +1814,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1787,7 +1859,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -1807,7 +1879,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:51:29
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1793,8 +1793,48 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Dank voor je interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 09:00 tot 18:00 uur. Op zaterdag zijn we geopend van 10:00 tot 16:00 uur. Op zondag zijn we gesloten. Mocht je verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:50:38</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1814,7 +1854,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1859,7 +1899,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:54:42
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1833,8 +1833,72 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:54:10</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:54:10</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1854,7 +1918,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1909,7 +1973,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:55:47
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1897,8 +1897,48 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw vraag. Onze openingstijden zijn maandag t/m vrijdag van 9:00 tot 17:00 uur. Op zaterdag zijn wij geopend van 10:00 tot 16:00 uur. Op zondag zijn wij gesloten.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:55:23</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1918,7 +1958,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1963,7 +2003,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:56:51
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1937,8 +1937,40 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:56:35</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1958,7 +1990,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2013,7 +2045,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:57:55
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1969,8 +1969,40 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:57:46</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1990,7 +2022,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2045,7 +2077,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 21:59:59
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2001,8 +2001,40 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-06-17 21:59:06</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2022,7 +2054,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2077,7 +2109,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:01:01
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2033,8 +2033,40 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:00:16</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2054,7 +2086,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2119,7 +2151,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:02:03
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2065,8 +2065,48 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Beste mevrouw/heer,
+Bedankt voor uw interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 09:00 tot 17:00 uur. Voor meer informatie kunt u onze website raadplegen of contact met ons opnemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:01:29</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2086,7 +2126,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2131,7 +2171,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:03:05
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2105,8 +2105,40 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:02:40</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2126,7 +2158,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G41">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2211,7 +2243,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:04:07
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,8 +2137,40 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:03:51</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2158,7 +2190,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G43">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2229,17 +2261,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:05:09
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2169,8 +2169,48 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Beste heer/mevrouw,
+Bedankt voor uw bericht. Onze openingstijden zijn maandag tot en met vrijdag van 9.00 uur tot 17.30 uur. Mocht u nog verdere vragen hebben, dan hoor ik het graag.
+Met vriendelijke groet,
+[Naam assistent]</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:05:03</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D43">
+  <conditionalFormatting sqref="D2:D44">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2190,7 +2230,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G43">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2235,7 +2275,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:07:13
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2209,8 +2209,40 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:06:14</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D44">
+  <conditionalFormatting sqref="D2:D45">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2230,7 +2262,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G44">
+  <conditionalFormatting sqref="G2:G45">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2295,7 +2327,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:08:15
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2241,8 +2241,40 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:07:25</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D45">
+  <conditionalFormatting sqref="D2:D46">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2262,7 +2294,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G45">
+  <conditionalFormatting sqref="G2:G46">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2327,7 +2359,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:09:18
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2273,8 +2273,40 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:08:36</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D2:D47">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2294,7 +2326,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G46">
+  <conditionalFormatting sqref="G2:G47">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2349,7 +2381,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:10:19
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2305,8 +2305,40 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:09:47</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D47">
+  <conditionalFormatting sqref="D2:D48">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2326,7 +2358,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G47">
+  <conditionalFormatting sqref="G2:G48">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2391,7 +2423,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:12:23
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2337,8 +2337,48 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Bedankt voor je vraag. Onze openingstijden zijn van maandag tot en met vrijdag van 09:00 tot 18:00 uur. Op zaterdag zijn we geopend van 10:00 tot 16:00 uur. Op zondag zijn we gesloten.
+Vriendelijke groet, 
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:12:09</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D48">
+  <conditionalFormatting sqref="D2:D49">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2358,7 +2398,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G48">
+  <conditionalFormatting sqref="G2:G49">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2403,7 +2443,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:13:25
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2377,8 +2377,40 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:13:20</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D49">
+  <conditionalFormatting sqref="D2:D50">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2398,7 +2430,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G2:G50">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2453,7 +2485,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:27:08
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2409,8 +2409,72 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:14:31</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:27:02</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D50">
+  <conditionalFormatting sqref="D2:D52">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2430,7 +2494,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G50">
+  <conditionalFormatting sqref="G2:G52">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2495,7 +2559,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -2505,7 +2569,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:29:11
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2473,8 +2473,72 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:29:05</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:29:05</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D52">
+  <conditionalFormatting sqref="D2:D54">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2494,7 +2558,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G52">
+  <conditionalFormatting sqref="G2:G54">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2549,7 +2613,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -2579,7 +2643,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:30:13
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2537,8 +2537,40 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:30:06</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D54">
+  <conditionalFormatting sqref="D2:D55">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2558,7 +2590,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G54">
+  <conditionalFormatting sqref="G2:G55">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2613,7 +2645,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:42:31
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2569,8 +2569,48 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 tot 17:00 uur. Op zondag zijn wij gesloten. Mocht u nog verdere vragen hebben, dan hoor ik dat graag.
+Met vriendelijke groet,
+[Naam van de assistent]</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:41:31</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D55">
+  <conditionalFormatting sqref="D2:D56">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2590,7 +2630,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G55">
+  <conditionalFormatting sqref="G2:G56">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2635,7 +2675,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:48:09
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2609,8 +2609,40 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:42:35</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D56">
+  <conditionalFormatting sqref="D2:D57">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2630,7 +2662,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G56">
+  <conditionalFormatting sqref="G2:G57">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2685,7 +2717,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:49:11
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2641,8 +2641,40 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:48:09</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D57">
+  <conditionalFormatting sqref="D2:D58">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2662,7 +2694,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G57">
+  <conditionalFormatting sqref="G2:G58">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2727,7 +2759,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 22:50:13
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2673,8 +2673,40 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:49:15</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D58">
+  <conditionalFormatting sqref="D2:D59">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2694,7 +2726,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G58">
+  <conditionalFormatting sqref="G2:G59">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2749,7 +2781,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 23:00:24
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2705,8 +2705,136 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:50:20</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:56:10</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:57:10</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2025-06-17 22:58:10</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D59">
+  <conditionalFormatting sqref="D2:D63">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2726,7 +2854,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G59">
+  <conditionalFormatting sqref="G2:G63">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2791,27 +2919,27 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 23:03:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2833,8 +2833,72 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2025-06-17 23:02:10</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>2025-06-17 23:02:11</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D63">
+  <conditionalFormatting sqref="D2:D65">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2854,7 +2918,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G63">
+  <conditionalFormatting sqref="G2:G65">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2909,7 +2973,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -2929,7 +2993,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-17 23:04:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2897,8 +2897,40 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>2025-06-17 23:03:10</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D65">
+  <conditionalFormatting sqref="D2:D66">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2918,7 +2950,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G65">
+  <conditionalFormatting sqref="G2:G66">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2973,7 +3005,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 08:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-17.xlsx
+++ b/logs/mail_log_2025-06-17.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2929,8 +2929,40 @@
         </is>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>2025-06-17 23:04:10</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D66">
+  <conditionalFormatting sqref="D2:D67">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2950,7 +2982,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G66">
+  <conditionalFormatting sqref="G2:G67">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3005,7 +3037,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">

</xml_diff>